<commit_message>
updated ref scoring spreadsheet. updated db-ERD. added base Circuit wireframe
</commit_message>
<xml_diff>
--- a/project-ref-files/EUCHRE-Scoring-Spreadsheet.xlsx
+++ b/project-ref-files/EUCHRE-Scoring-Spreadsheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryansage/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryansage/sei-course/ga-sei/euchre500/project-ref-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA4524E-13FA-4648-ADF4-2AB775603271}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1CC375-2D07-C548-99AB-06E54B4106F9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56620" yWindow="3300" windowWidth="10580" windowHeight="14700" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20480" windowHeight="14900" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TM v DW" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,10 @@
     <sheet name="FIRST 500" sheetId="4" r:id="rId4"/>
     <sheet name="NEXT 500" sheetId="5" r:id="rId5"/>
     <sheet name="The Next Next 500" sheetId="6" r:id="rId6"/>
-    <sheet name="The Next Next, Next 500" sheetId="7" r:id="rId7"/>
-    <sheet name="The Next Next Next, Next 500" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet1 (2)" sheetId="10" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId8"/>
+    <sheet name="The Next Next, Next 500" sheetId="7" r:id="rId9"/>
+    <sheet name="The Next Next Next, Next 500" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -170,6 +172,114 @@
   <si>
     <t xml:space="preserve">WIN </t>
   </si>
+  <si>
+    <t>tScore</t>
+  </si>
+  <si>
+    <t>tLoaners</t>
+  </si>
+  <si>
+    <t>tEuchres</t>
+  </si>
+  <si>
+    <t>tMarchs</t>
+  </si>
+  <si>
+    <t>tLose</t>
+  </si>
+  <si>
+    <t>tWin</t>
+  </si>
+  <si>
+    <t>tRounds</t>
+  </si>
+  <si>
+    <t>Model: Circuits - Keeps tally of rScores once submitted</t>
+  </si>
+  <si>
+    <t>player4</t>
+  </si>
+  <si>
+    <t>player1</t>
+  </si>
+  <si>
+    <t>player2</t>
+  </si>
+  <si>
+    <t>player3</t>
+  </si>
+  <si>
+    <t>Teams</t>
+  </si>
+  <si>
+    <t>M+D</t>
+  </si>
+  <si>
+    <t>T+W</t>
+  </si>
+  <si>
+    <t>W+D</t>
+  </si>
+  <si>
+    <t>T+M</t>
+  </si>
+  <si>
+    <t>T+D</t>
+  </si>
+  <si>
+    <t>W+M</t>
+  </si>
+  <si>
+    <t>p1+p2</t>
+  </si>
+  <si>
+    <t>p3+p4</t>
+  </si>
+  <si>
+    <t>p1+p3</t>
+  </si>
+  <si>
+    <t>p2+p4</t>
+  </si>
+  <si>
+    <t>p4+p1</t>
+  </si>
+  <si>
+    <t>p2+p3</t>
+  </si>
+  <si>
+    <t>rScore</t>
+  </si>
+  <si>
+    <t>rLoaner</t>
+  </si>
+  <si>
+    <t>rEuchres</t>
+  </si>
+  <si>
+    <t>rMarchs</t>
+  </si>
+  <si>
+    <t>rWin</t>
+  </si>
+  <si>
+    <t>rLose</t>
+  </si>
+  <si>
+    <t>Model: rScore - after each hand (aka trick), scores are entered. Send will push values up to Circuits. R</t>
+  </si>
+  <si>
+    <t>Model: rScore - after each hand (aka trick), scores are entered. Send will push values up to Circuits. tRounds is updated on each round submit</t>
+  </si>
+  <si>
+    <t>"submit"</t>
+  </si>
+  <si>
+    <t>teams are auto create around pairing each player together, as shown above</t>
+  </si>
+  <si>
+    <t>Model: Circuits - Keeps individual score tally of teams rScores once submitted</t>
+  </si>
 </sst>
 </file>
 
@@ -179,7 +289,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -273,8 +383,58 @@
       <sz val="18"/>
       <name val="Century Gothic"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -323,8 +483,20 @@
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -347,11 +519,328 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -592,6 +1081,106 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -943,6 +1532,318 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rounded Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28D11B18-10CD-0C4E-8F23-B57D8E0A5242}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8432800" y="939800"/>
+          <a:ext cx="927100" cy="241300"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Start</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Circuit</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rounded Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4F5E51B-84C2-FA4A-BE44-F2E2327D141D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8712200" y="700617"/>
+          <a:ext cx="927100" cy="245533"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Start</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Circuit</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>84666</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>21167</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1011766</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>97366</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rounded Rectangle 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F68C887-73FF-EB44-8FEB-298FA4C4A083}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="910166" y="190500"/>
+          <a:ext cx="927100" cy="245533"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>add player</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>687916</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>137583</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>296332</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>138430</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Line Callout 1 (Border and Accent Bar) 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1865B16-0C22-354B-ADB7-EA31B6BFDC85}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10149416" y="1852083"/>
+          <a:ext cx="1259416" cy="868680"/>
+        </a:xfrm>
+        <a:prstGeom prst="accentBorderCallout1">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 91849"/>
+            <a:gd name="adj2" fmla="val -11694"/>
+            <a:gd name="adj3" fmla="val 86892"/>
+            <a:gd name="adj4" fmla="val -57662"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Add Score: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>3 hidden fields</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>P1:_id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>P2:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> _id</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1245,7 +2146,7 @@
   </sheetPr>
   <dimension ref="A1:R132"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -5496,6 +6397,150 @@
       <formula>"Tyler"</formula>
     </cfRule>
   </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="82" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="82" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="82" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="82" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="82" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="84">
+        <f>SUM('TM v DW'!B132+'TM v DW'!C132+'TM v DW'!H132+'TM v DW'!I132+'TW v MD'!B136+'TW v MD'!C136+'TW v MD'!H136+'TW v MD'!I136+'TD v MW'!B142+'TD v MW'!C142+'TD v MW'!H142+'TD v MW'!I142+E2)</f>
+        <v>508</v>
+      </c>
+      <c r="C2" s="84">
+        <f>SUM('TM v DW'!C132+'TW v MD'!C136+'TD v MW'!C142)</f>
+        <v>11</v>
+      </c>
+      <c r="D2" s="84">
+        <f>SUM('TM v DW'!I132+'TW v MD'!I136+'TD v MW'!I142)</f>
+        <v>29</v>
+      </c>
+      <c r="E2" s="84">
+        <f>SUM('TM v DW'!F132+'TW v MD'!F136+'TD v MW'!F142)</f>
+        <v>29</v>
+      </c>
+      <c r="F2" s="84">
+        <f>SUM('TM v DW'!H132+'TW v MD'!H136+'TD v MW'!H142)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="84">
+        <f>SUM('TM v DW'!L132+'TM v DW'!M132+'TM v DW'!P132+'TM v DW'!Q132+'TW v MD'!D136+'TW v MD'!E136+'TW v MD'!H136+'TW v MD'!I136+'TD v MW'!L142+'TD v MW'!M142+'TD v MW'!P142+'TD v MW'!Q142+E3)</f>
+        <v>488</v>
+      </c>
+      <c r="C3" s="84">
+        <f>SUM('TM v DW'!M132+'TW v MD'!E136+'TD v MW'!M142)</f>
+        <v>14</v>
+      </c>
+      <c r="D3" s="84">
+        <f>SUM('TM v DW'!Q132+'TW v MD'!I136+'TD v MW'!Q142)</f>
+        <v>24</v>
+      </c>
+      <c r="E3" s="84">
+        <f>SUM('TM v DW'!N132+'TW v MD'!F136+'TD v MW'!N142)</f>
+        <v>21</v>
+      </c>
+      <c r="F3" s="83">
+        <f>SUM('TM v DW'!P132+'TW v MD'!H136+'TD v MW'!P142)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="83" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="84">
+        <f>SUM('TM v DW'!D132+'TM v DW'!E132+'TM v DW'!H132+'TM v DW'!I132+'TW v MD'!J136+'TW v MD'!K136+'TW v MD'!P136+'TW v MD'!Q136+'TD v MW'!J142+'TD v MW'!K142+'TD v MW'!P142+'TD v MW'!Q142+E4)</f>
+        <v>482</v>
+      </c>
+      <c r="C4" s="84">
+        <f>SUM('TM v DW'!E132+'TW v MD'!K136+'TD v MW'!K142)</f>
+        <v>14</v>
+      </c>
+      <c r="D4" s="84">
+        <f>SUM('TM v DW'!I132+'TW v MD'!Q136+'TD v MW'!Q142)</f>
+        <v>29</v>
+      </c>
+      <c r="E4" s="84">
+        <f>SUM('TM v DW'!F132+'TW v MD'!N136+'TD v MW'!N142)</f>
+        <v>24</v>
+      </c>
+      <c r="F4" s="84">
+        <f>SUM('TM v DW'!H132+'TW v MD'!P136+'TD v MW'!P142)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="83" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="84">
+        <f>SUM('TM v DW'!J132+'TM v DW'!K132+'TM v DW'!P132+'TM v DW'!Q132+'TW v MD'!L136+'TW v MD'!M136+'TW v MD'!P136+'TW v MD'!Q136+'TD v MW'!D142+'TD v MW'!E142+'TD v MW'!H142+'TD v MW'!I142+E5)</f>
+        <v>480</v>
+      </c>
+      <c r="C5" s="84">
+        <f>SUM('TM v DW'!K132+'TW v MD'!M136+'TD v MW'!E142)</f>
+        <v>3</v>
+      </c>
+      <c r="D5" s="84">
+        <f>SUM('TM v DW'!Q132+'TW v MD'!Q136+'TD v MW'!I142)</f>
+        <v>30</v>
+      </c>
+      <c r="E5" s="84">
+        <f>SUM('TM v DW'!N132+'TW v MD'!N136+'TD v MW'!F142)</f>
+        <v>26</v>
+      </c>
+      <c r="F5" s="84">
+        <f>SUM('TM v DW'!P132+'TW v MD'!P136+'TD v MW'!H142)</f>
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -69804,8 +70849,8 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -69923,8 +70968,8 @@
   </sheetPr>
   <dimension ref="A21:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -70055,6 +71100,613 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A81E2EA-82EE-9A49-8EC7-A8A50854F2A1}">
+  <dimension ref="A3:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="8" max="8" width="30.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B4" s="86" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="88"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B5" s="89"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="91" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B6" s="92" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="80" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="93" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" s="100" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="51">
+        <f>SUM('TW v MD'!B63+'TW v MD'!C63+'TW v MD'!H63+'TW v MD'!I63+'TM v DW'!B51+'TM v DW'!C51+'TM v DW'!H51+'TM v DW'!I51+'TD v MW'!B65+'TD v MW'!C65+'TD v MW'!H65+'TD v MW'!I65)</f>
+        <v>25</v>
+      </c>
+      <c r="D7" s="51">
+        <f>SUM('TM v DW'!C51+'TW v MD'!C63+'TD v MW'!C65)</f>
+        <v>1</v>
+      </c>
+      <c r="E7" s="29">
+        <f>SUM('TM v DW'!E51+'TW v MD'!E63+'TD v MW'!E65)</f>
+        <v>1</v>
+      </c>
+      <c r="F7" s="51">
+        <f>SUM('TM v DW'!I51+'TW v MD'!I63+'TD v MW'!I65)</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="51">
+        <f>SUM('TM v DW'!F51+'TW v MD'!F63+'TD v MW'!F65)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="95">
+        <f>SUM('TM v DW'!H51+'TW v MD'!H63+'TD v MW'!H65)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="100" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="94" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="51">
+        <f>SUM('TM v DW'!L51+'TM v DW'!M51+'TM v DW'!P51+'TM v DW'!Q51+'TW v MD'!D63+'TW v MD'!E63+'TW v MD'!H63+'TW v MD'!I63+'TD v MW'!L65+'TD v MW'!M65+'TD v MW'!P65+'TD v MW'!Q65)</f>
+        <v>22</v>
+      </c>
+      <c r="D8" s="51">
+        <f>SUM('TM v DW'!M51+'TW v MD'!E63+'TD v MW'!M65)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="29">
+        <f>SUM('TM v DW'!M51+'TW v MD'!E63+'TD v MW'!M65)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="51">
+        <f>SUM('TM v DW'!Q51+'TW v MD'!I63+'TD v MW'!Q65)</f>
+        <v>3</v>
+      </c>
+      <c r="G8" s="51">
+        <f>SUM('TM v DW'!N51+'TW v MD'!F63+'TD v MW'!N65)</f>
+        <v>1</v>
+      </c>
+      <c r="H8" s="95">
+        <f>SUM('TM v DW'!P51+'TW v MD'!H63+'TD v MW'!P65)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A9" s="100" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="51">
+        <f>SUM('TM v DW'!D51+'TM v DW'!E51+'TM v DW'!H51+'TM v DW'!I51+'TW v MD'!J63+'TW v MD'!K63+'TW v MD'!P63+'TW v MD'!Q63)+'TD v MW'!J65+'TD v MW'!K65+'TD v MW'!P65+'TD v MW'!Q65</f>
+        <v>38</v>
+      </c>
+      <c r="D9" s="51">
+        <f>SUM('TM v DW'!E51+'TW v MD'!K63+'TD v MW'!K65)</f>
+        <v>2</v>
+      </c>
+      <c r="E9" s="29">
+        <f>SUM('TM v DW'!E51+'TW v MD'!M63+'TD v MW'!M65)</f>
+        <v>1</v>
+      </c>
+      <c r="F9" s="51">
+        <f>SUM('TM v DW'!I51+'TW v MD'!Q63+'TD v MW'!Q65)</f>
+        <v>3</v>
+      </c>
+      <c r="G9" s="51">
+        <f>SUM('TM v DW'!F51+'TW v MD'!N63+'TD v MW'!N65)</f>
+        <v>2</v>
+      </c>
+      <c r="H9" s="95">
+        <f>SUM('TM v DW'!H51+'TW v MD'!P63+'TD v MW'!P65)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="100" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="96" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="97">
+        <f>SUM('TM v DW'!J51+'TM v DW'!K51+'TM v DW'!P51+'TM v DW'!Q51+'TW v MD'!L63+'TW v MD'!M63+'TW v MD'!P63+'TW v MD'!Q63+'TD v MW'!D65+'TD v MW'!E65+'TD v MW'!H65+'TD v MW'!I65)</f>
+        <v>18</v>
+      </c>
+      <c r="D10" s="97">
+        <f>SUM('TM v DW'!K51+'TW v MD'!M63+'TD v MW'!E65)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="98">
+        <f>SUM('TM v DW'!M51+'TW v MD'!M63+'TD v MW'!E65)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" s="97">
+        <f>SUM('TM v DW'!Q51+'TW v MD'!Q63+'TD v MW'!Q65)</f>
+        <v>4</v>
+      </c>
+      <c r="G10" s="97">
+        <f>SUM('TM v DW'!N51+'TW v MD'!N63+'TD v MW'!F65)</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="99">
+        <f>SUM('TM v DW'!P51+'TW v MD'!P63+'TD v MW'!H65)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B13" s="86" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="87"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="88"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B14" s="89"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="101"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="B15" s="105" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="102" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="112" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="113" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="114" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="102" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="115" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A16" s="100" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="106" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="103"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="107"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A17" s="100" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="106" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="103"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="107"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A18" s="100" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="106" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="103"/>
+      <c r="D18" s="103"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="103"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="107"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A19" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="106" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="103"/>
+      <c r="D19" s="103"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="107"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A20" s="100" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="106" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="103"/>
+      <c r="D20" s="103"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="107"/>
+    </row>
+    <row r="21" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="100" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="108" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="109"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="110"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="109"/>
+      <c r="H21" s="111"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B13:H13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35ADD392-0E8E-6C46-9EAC-E0F36BEF3962}">
+  <dimension ref="A3:I23"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="32.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B4" s="86" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="87"/>
+      <c r="D4" s="87"/>
+      <c r="E4" s="87"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="87"/>
+      <c r="H4" s="88"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B5" s="89"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="90"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="91" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B6" s="92" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="80" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="93" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A7" s="100" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="94" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="95"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A8" s="100" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="94" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="95"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A9" s="100" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="94" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="95"/>
+    </row>
+    <row r="10" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="100" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="96" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="97"/>
+      <c r="D10" s="97"/>
+      <c r="E10" s="98"/>
+      <c r="F10" s="97"/>
+      <c r="G10" s="97"/>
+      <c r="H10" s="99"/>
+    </row>
+    <row r="12" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B13" s="86" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="87"/>
+      <c r="D13" s="87"/>
+      <c r="E13" s="87"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="88"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B14" s="89"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="101"/>
+    </row>
+    <row r="15" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="105" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="102" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="112" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="113" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="114" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="102" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="115" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A16" s="100" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="106" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="103"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="104"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="116"/>
+      <c r="I16" s="120" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17" s="100" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="106" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="103"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="104"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="116"/>
+      <c r="I17" s="121" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A18" s="100" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="106" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="103"/>
+      <c r="D18" s="103"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="103"/>
+      <c r="G18" s="103"/>
+      <c r="H18" s="116"/>
+      <c r="I18" s="121" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A19" s="100" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="106" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="103"/>
+      <c r="D19" s="103"/>
+      <c r="E19" s="104"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="103"/>
+      <c r="H19" s="116"/>
+      <c r="I19" s="121" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A20" s="100" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="106" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="103"/>
+      <c r="D20" s="103"/>
+      <c r="E20" s="104"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="103"/>
+      <c r="H20" s="116"/>
+      <c r="I20" s="121" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="100" t="s">
+        <v>68</v>
+      </c>
+      <c r="B21" s="108" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" s="109"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="110"/>
+      <c r="F21" s="109"/>
+      <c r="G21" s="109"/>
+      <c r="H21" s="117"/>
+      <c r="I21" s="122" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A23" s="118" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="119"/>
+      <c r="C23" s="119"/>
+      <c r="D23" s="119"/>
+      <c r="E23" s="119"/>
+      <c r="F23" s="119"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B13:H13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -70188,148 +71840,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:F5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.83203125" customWidth="1"/>
-    <col min="5" max="5" width="8.5" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="82" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="82" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="82" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="82" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="82" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="84">
-        <f>SUM('TM v DW'!B132+'TM v DW'!C132+'TM v DW'!H132+'TM v DW'!I132+'TW v MD'!B136+'TW v MD'!C136+'TW v MD'!H136+'TW v MD'!I136+'TD v MW'!B142+'TD v MW'!C142+'TD v MW'!H142+'TD v MW'!I142+E2)</f>
-        <v>508</v>
-      </c>
-      <c r="C2" s="84">
-        <f>SUM('TM v DW'!C132+'TW v MD'!C136+'TD v MW'!C142)</f>
-        <v>11</v>
-      </c>
-      <c r="D2" s="84">
-        <f>SUM('TM v DW'!I132+'TW v MD'!I136+'TD v MW'!I142)</f>
-        <v>29</v>
-      </c>
-      <c r="E2" s="84">
-        <f>SUM('TM v DW'!F132+'TW v MD'!F136+'TD v MW'!F142)</f>
-        <v>29</v>
-      </c>
-      <c r="F2" s="84">
-        <f>SUM('TM v DW'!H132+'TW v MD'!H136+'TD v MW'!H142)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="84">
-        <f>SUM('TM v DW'!L132+'TM v DW'!M132+'TM v DW'!P132+'TM v DW'!Q132+'TW v MD'!D136+'TW v MD'!E136+'TW v MD'!H136+'TW v MD'!I136+'TD v MW'!L142+'TD v MW'!M142+'TD v MW'!P142+'TD v MW'!Q142+E3)</f>
-        <v>488</v>
-      </c>
-      <c r="C3" s="84">
-        <f>SUM('TM v DW'!M132+'TW v MD'!E136+'TD v MW'!M142)</f>
-        <v>14</v>
-      </c>
-      <c r="D3" s="84">
-        <f>SUM('TM v DW'!Q132+'TW v MD'!I136+'TD v MW'!Q142)</f>
-        <v>24</v>
-      </c>
-      <c r="E3" s="84">
-        <f>SUM('TM v DW'!N132+'TW v MD'!F136+'TD v MW'!N142)</f>
-        <v>21</v>
-      </c>
-      <c r="F3" s="83">
-        <f>SUM('TM v DW'!P132+'TW v MD'!H136+'TD v MW'!P142)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="83" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="84">
-        <f>SUM('TM v DW'!D132+'TM v DW'!E132+'TM v DW'!H132+'TM v DW'!I132+'TW v MD'!J136+'TW v MD'!K136+'TW v MD'!P136+'TW v MD'!Q136+'TD v MW'!J142+'TD v MW'!K142+'TD v MW'!P142+'TD v MW'!Q142+E4)</f>
-        <v>482</v>
-      </c>
-      <c r="C4" s="84">
-        <f>SUM('TM v DW'!E132+'TW v MD'!K136+'TD v MW'!K142)</f>
-        <v>14</v>
-      </c>
-      <c r="D4" s="84">
-        <f>SUM('TM v DW'!I132+'TW v MD'!Q136+'TD v MW'!Q142)</f>
-        <v>29</v>
-      </c>
-      <c r="E4" s="84">
-        <f>SUM('TM v DW'!F132+'TW v MD'!N136+'TD v MW'!N142)</f>
-        <v>24</v>
-      </c>
-      <c r="F4" s="84">
-        <f>SUM('TM v DW'!H132+'TW v MD'!P136+'TD v MW'!P142)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="83" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="84">
-        <f>SUM('TM v DW'!J132+'TM v DW'!K132+'TM v DW'!P132+'TM v DW'!Q132+'TW v MD'!L136+'TW v MD'!M136+'TW v MD'!P136+'TW v MD'!Q136+'TD v MW'!D142+'TD v MW'!E142+'TD v MW'!H142+'TD v MW'!I142+E5)</f>
-        <v>480</v>
-      </c>
-      <c r="C5" s="84">
-        <f>SUM('TM v DW'!K132+'TW v MD'!M136+'TD v MW'!E142)</f>
-        <v>3</v>
-      </c>
-      <c r="D5" s="84">
-        <f>SUM('TM v DW'!Q132+'TW v MD'!Q136+'TD v MW'!I142)</f>
-        <v>30</v>
-      </c>
-      <c r="E5" s="84">
-        <f>SUM('TM v DW'!N132+'TW v MD'!N136+'TD v MW'!F142)</f>
-        <v>26</v>
-      </c>
-      <c r="F5" s="84">
-        <f>SUM('TM v DW'!P132+'TW v MD'!P136+'TD v MW'!H142)</f>
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>